<commit_message>
update data and photo
</commit_message>
<xml_diff>
--- a/data/car_data.xlsx
+++ b/data/car_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinhsieh/luxgen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2B0FA5-5E36-5340-BD21-1898CD55D068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E28470-675D-1A40-8907-E99E65088BF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="20000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="200">
   <si>
     <t>C71</t>
   </si>
@@ -764,7 +764,10 @@
     <t>2021/11</t>
   </si>
   <si>
-    <t>2021/01-11</t>
+    <t>2021/12</t>
+  </si>
+  <si>
+    <t>2021</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1425,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1529,9 +1532,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12712,11 +12712,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C3EFB7-4E46-D14F-BDDF-05073EF0410F}">
-  <dimension ref="A1:J149"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F155" sqref="F155"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -15225,7 +15225,7 @@
         <v>184</v>
       </c>
       <c r="H139" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J139" s="10">
         <v>457</v>
@@ -15369,6 +15369,17 @@
       </c>
       <c r="J149" s="10">
         <v>109</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="A150" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="G150" s="10">
+        <v>83</v>
+      </c>
+      <c r="J150" s="10">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -15383,7 +15394,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -15423,7 +15434,7 @@
       </c>
       <c r="C3" s="16">
         <f>SUM(dataI!G2:G150)</f>
-        <v>40754</v>
+        <v>40837</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15447,7 +15458,7 @@
       </c>
       <c r="C5" s="16">
         <f>SUM(dataI!J2:J150)</f>
-        <v>4089</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -15495,7 +15506,7 @@
       </c>
       <c r="C9" s="16">
         <f>SUM(dataI!H2:H150)</f>
-        <v>6161</v>
+        <v>6164</v>
       </c>
     </row>
   </sheetData>
@@ -15509,7 +15520,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -15832,7 +15843,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="35" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E14" s="16">
         <f>SUM(dataI!E139:E150)</f>
@@ -15840,15 +15851,15 @@
       </c>
       <c r="G14" s="16">
         <f>SUM(dataI!G139:G150)</f>
-        <v>1152</v>
+        <v>1235</v>
       </c>
       <c r="H14" s="16">
         <f>SUM(dataI!H139:H150)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J14" s="16">
         <f>SUM(dataI!J139:J150)</f>
-        <v>1658</v>
+        <v>1829</v>
       </c>
     </row>
   </sheetData>
@@ -15862,7 +15873,7 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -16246,25 +16257,25 @@
       <c r="U13" s="26"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="36" t="s">
-        <v>198</v>
+      <c r="A14" s="16">
+        <v>2021</v>
       </c>
       <c r="B14" s="28">
         <f>SUM(dataIII!B14:J14)</f>
-        <v>3680</v>
+        <v>3937</v>
       </c>
       <c r="C14" s="33">
-        <v>25395</v>
+        <v>28049</v>
       </c>
       <c r="D14" s="33">
-        <v>21898</v>
+        <v>24650</v>
       </c>
       <c r="E14" s="34">
         <f t="shared" si="0"/>
-        <v>0.89854279798413872</v>
+        <v>0.87516310666230968</v>
       </c>
       <c r="F14" s="33">
-        <v>409552</v>
+        <v>449859</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -17234,8 +17245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B7988E-8DD6-4053-A351-E3512FCFE7D0}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -17772,8 +17783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA1D382-D570-428C-8F19-6194B60E3445}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>

</xml_diff>